<commit_message>
new api for flights added, and testing to see whats wrong, and why im getting 404 errors. changed the api key and still getting erros
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -1,38 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEE6CF2-2B61-47AC-8B72-6C50114A97E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E5920C-B776-403B-BFF5-6FA17481AED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>date</t>
   </si>
   <si>
-    <t>time spend</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -142,6 +150,18 @@
   </si>
   <si>
     <t>I managed to get the weather api to work, and the passport requirements api, so we are good to go on integrating backend and front end</t>
+  </si>
+  <si>
+    <t>Amadeus API does not work, because something is wrong with the API key, I looked at all the documentation, and I'm trying to implement some other API so hopefully solve my issues. I tried to debug it, but it kept giving a token not found error.</t>
+  </si>
+  <si>
+    <t>time spent</t>
+  </si>
+  <si>
+    <t>implemented a new flight API from the aviation stack, however, I'm still getting the same errors as before where the im getting HTTP 404 not found</t>
+  </si>
+  <si>
+    <t>reading and figured the issue could be my access point or my api key so I tried to get a new api key and that didn’t help, so I'm going to try a new access point</t>
   </si>
 </sst>
 </file>
@@ -461,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="139" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,10 +499,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -493,7 +513,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -504,7 +524,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -515,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -526,7 +546,7 @@
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -537,7 +557,7 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -545,7 +565,7 @@
         <v>45180</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -556,7 +576,7 @@
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -567,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -578,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -589,7 +609,7 @@
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -597,7 +617,7 @@
         <v>45187</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -608,7 +628,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -619,7 +639,7 @@
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -630,7 +650,7 @@
         <v>6</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -641,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -652,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -663,7 +683,7 @@
         <v>3</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -674,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -685,7 +705,7 @@
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -696,7 +716,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -707,7 +727,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -718,7 +738,7 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -729,7 +749,7 @@
         <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -740,12 +760,12 @@
         <v>5</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -756,7 +776,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -767,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -778,7 +798,7 @@
         <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -789,7 +809,7 @@
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -800,15 +820,15 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C37" t="s">
         <v>33</v>
-      </c>
-      <c r="C37" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -819,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -830,7 +850,7 @@
         <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -841,7 +861,7 @@
         <v>5</v>
       </c>
       <c r="C41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -852,7 +872,40 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>45229</v>
+      </c>
+      <c r="B43">
+        <v>2</v>
+      </c>
+      <c r="C43" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>45232</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
+        <v>45235</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a new APi for the flight data, a bunch of new errors have spawned and I have no idea what to do, hopefully I can reconsile this
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E5920C-B776-403B-BFF5-6FA17481AED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DE7283-1C64-434B-9C17-D034173A96F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>date</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>reading and figured the issue could be my access point or my api key so I tried to get a new api key and that didn’t help, so I'm going to try a new access point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I changed the API one more time for the flight data to open sky API But some of the imports werent working so I had to do some research and find where the JAR files are. 2 of the imports are still erroring, and I don’t know where to find the JAR file for it. </t>
   </si>
 </sst>
 </file>
@@ -481,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -908,6 +911,17 @@
         <v>41</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>45237</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
debugging dependencies is really stressing me out, I have used 3 different APIs that have been giving me issues, this skyscanner import isnt working
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0DE7283-1C64-434B-9C17-D034173A96F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0E2CEE-1EF3-4A17-A7B9-538FEACC209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>date</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t xml:space="preserve">I changed the API one more time for the flight data to open sky API But some of the imports werent working so I had to do some research and find where the JAR files are. 2 of the imports are still erroring, and I don’t know where to find the JAR file for it. </t>
+  </si>
+  <si>
+    <t>With the flight scanner API, an API that tracks flight data, the issue is two of the imports don’t work, Ive been searching everywhere on stack overflow, looking on the documentation, and reading, and still cant find a solution. One of the things I tried was deleting, and re-importing all of the dependencies of the project, However, when i ran the code it tells me other imports arent working</t>
   </si>
 </sst>
 </file>
@@ -484,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="105" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,6 +925,17 @@
         <v>42</v>
       </c>
     </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>45239</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
putting the SkyScannerAPI idea on hold, I think im just going to have someone input their data into a window, srarted the code for that
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0E2CEE-1EF3-4A17-A7B9-538FEACC209B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DBE89-E987-402C-B484-20B2E2A44E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>date</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>With the flight scanner API, an API that tracks flight data, the issue is two of the imports don’t work, Ive been searching everywhere on stack overflow, looking on the documentation, and reading, and still cant find a solution. One of the things I tried was deleting, and re-importing all of the dependencies of the project, However, when i ran the code it tells me other imports arent working</t>
+  </si>
+  <si>
+    <t>so I tried to go back and use the other API, skyScanner API, so I went looking for the jar file since that was what was wrong.I couldn’t find so I thought maybe I could add it as a depenedency, but no I crashed the while prpgram again, and had to re-install all the other HTTP jar files. InteleJ is not good</t>
+  </si>
+  <si>
+    <t>I put the dream of having a flight api aside, and Im just going to have someone input their data into the a little window that’s going to popup, I added the code to my controller class</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -936,6 +942,28 @@
         <v>43</v>
       </c>
     </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>45241</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>45242</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
debugging UI, FXML and controller class debug, also starting frontend and backend integration
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DBE89-E987-402C-B484-20B2E2A44E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E0529E-B35E-4AB9-8D66-EC7B5C3E16FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>date</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>I put the dream of having a flight api aside, and Im just going to have someone input their data into the a little window that’s going to popup, I added the code to my controller class</t>
+  </si>
+  <si>
+    <t>bebugging ie some of the FXML and the controller integration class werent working properly, and data wasn’t being printed</t>
+  </si>
+  <si>
+    <t>starting the back-end and frontend UI integrations with the APIS, and front end</t>
   </si>
 </sst>
 </file>
@@ -493,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -964,6 +970,28 @@
         <v>45</v>
       </c>
     </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>45244</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>45246</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
debugging+ figuring out ways to implement api to frontend+ integrated budget panel
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E0529E-B35E-4AB9-8D66-EC7B5C3E16FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1BDF77-14FD-4B36-897C-1818CE864336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>date</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>starting the back-end and frontend UI integrations with the APIS, and front end</t>
+  </si>
+  <si>
+    <t>started implementing the integration between the front end and back, starting with printing the travel advisories on the panels on the UI section&lt; but its still very buggy and it doesn’t work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">debugging integrations between frontend and backend, thinking either sending everything to database then fetching, just printing it all out front. </t>
+  </si>
+  <si>
+    <t>budget panel frontend and backend integrated however, the code is still buggy, continuing to work on it</t>
   </si>
 </sst>
 </file>
@@ -499,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -992,6 +1001,39 @@
         <v>47</v>
       </c>
     </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
+        <v>45247</v>
+      </c>
+      <c r="B54">
+        <v>3</v>
+      </c>
+      <c r="C54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>45248</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
+      </c>
+      <c r="C56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>45249</v>
+      </c>
+      <c r="B57">
+        <v>4</v>
+      </c>
+      <c r="C57" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
re-coded the budget panel, but still having issues
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A1BDF77-14FD-4B36-897C-1818CE864336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF339E3-BA56-4E00-8CD8-3DD8C685199C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>date</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>budget panel frontend and backend integrated however, the code is still buggy, continuing to work on it</t>
+  </si>
+  <si>
+    <t>github messed up with the merging with the main and master class. So my code didn’t run so I had to fix the issue. I did a lot of research and debugging, I had to delete the .idea folder, and it worked</t>
+  </si>
+  <si>
+    <t>the budget panel code got taken out because of the github issues, so I had to re-do it, but the code has issues in it</t>
   </si>
 </sst>
 </file>
@@ -508,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A36" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1034,6 +1040,28 @@
         <v>50</v>
       </c>
     </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>45250</v>
+      </c>
+      <c r="B58">
+        <v>4</v>
+      </c>
+      <c r="C58" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>45252</v>
+      </c>
+      <c r="B59">
+        <v>3</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
I fized all of the bugs of the budget class and started on api-frontend integration
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD93B50-89F8-4707-969E-C9263DD43557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0A9A5-B657-4133-93E7-DABA3FFAFD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>date</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>budget panel code complete, few errors but it prints values</t>
+  </si>
+  <si>
+    <t>debugged the budget panel code and it works perfectly fine now. I started on the code for the api frontend integration</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C61"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1090,6 +1093,17 @@
         <v>54</v>
       </c>
     </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>45256</v>
+      </c>
+      <c r="B63">
+        <v>3</v>
+      </c>
+      <c r="C63" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
weatheAPI and frontend having some errors, trying to fix now
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F0A9A5-B657-4133-93E7-DABA3FFAFD8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3A6430-4F3F-4AB8-9958-CA5E0FA7B812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>date</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>debugged the budget panel code and it works perfectly fine now. I started on the code for the api frontend integration</t>
+  </si>
+  <si>
+    <t>intergrating the travel advisory with the front-end was still giving me a lot of errors, so now im working on the integration woth the weather api, but this is giving a lot of errors as well</t>
   </si>
 </sst>
 </file>
@@ -523,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C63"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
+      <selection activeCell="C64" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1104,6 +1107,17 @@
         <v>55</v>
       </c>
     </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>45258</v>
+      </c>
+      <c r="B64">
+        <v>4</v>
+      </c>
+      <c r="C64" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added the visarequirements printing class, and its really buggy, but im going to fix it
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3A6430-4F3F-4AB8-9958-CA5E0FA7B812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544FE37-3045-4D4F-ADE5-6A294F7D26A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>date</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>intergrating the travel advisory with the front-end was still giving me a lot of errors, so now im working on the integration woth the weather api, but this is giving a lot of errors as well</t>
+  </si>
+  <si>
+    <t>the visa requirements frontend implementation is giving some errors but im trying to fix it</t>
   </si>
 </sst>
 </file>
@@ -526,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C64"/>
+  <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,6 +1121,17 @@
         <v>56</v>
       </c>
     </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>45259</v>
+      </c>
+      <c r="B65">
+        <v>3</v>
+      </c>
+      <c r="C65" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
wearher API intergration complete, and almost done with the visa requiirement API
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7544FE37-3045-4D4F-ADE5-6A294F7D26A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E647C5-4A81-4AE3-89DC-B49753C5402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>date</t>
   </si>
@@ -210,6 +210,12 @@
   </si>
   <si>
     <t>the visa requirements frontend implementation is giving some errors but im trying to fix it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trying to debug the visa requirements intergaration with the </t>
+  </si>
+  <si>
+    <t>got the weather API intergrated into the UI, and have the VISA requirements almost working</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C65"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1132,6 +1138,28 @@
         <v>57</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B66">
+        <v>3</v>
+      </c>
+      <c r="C66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="2">
+        <v>45262</v>
+      </c>
+      <c r="B67">
+        <v>5</v>
+      </c>
+      <c r="C67" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
this is my last commit, there have been many changes since my last commit, but i havent pushed anything since DEC 2nd but there was alot of progress
</commit_message>
<xml_diff>
--- a/TIME_LOG_4900.xlsx
+++ b/TIME_LOG_4900.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waeld\Travel_inten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E647C5-4A81-4AE3-89DC-B49753C5402C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71262014-A441-46FE-86D9-BC1AAC9BA597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>date</t>
   </si>
@@ -216,6 +216,9 @@
   </si>
   <si>
     <t>got the weather API intergrated into the UI, and have the VISA requirements almost working</t>
+  </si>
+  <si>
+    <t>since the last update I made  a whole bunch of changes but I forgot to update them on the time log but check the github, a lot of things were added</t>
   </si>
 </sst>
 </file>
@@ -535,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="103" zoomScaleNormal="386" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1160,6 +1163,14 @@
         <v>59</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68" s="2">
+        <v>45273</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>